<commit_message>
just resaved the excel sheet
</commit_message>
<xml_diff>
--- a/data/Developed.Developing.xlsx
+++ b/data/Developed.Developing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="300" yWindow="-22600" windowWidth="28540" windowHeight="22320" tabRatio="500"/>
+    <workbookView xWindow="260" yWindow="440" windowWidth="28540" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -581,7 +581,7 @@
   <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+      <selection activeCell="B64" activeCellId="15" sqref="B4:B5 B7:B8 B11 B17:B18 B21 B23:B24 B26 B28:B29 B32:B34 B36 B46:B47 B50 B52:B55 B57 B59:B62 B64:B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>